<commit_message>
Atu 16 17 18
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos.xlsx
+++ b/Artefatos/17. Análise dos Eventos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28B08333-A05C-4F72-9E1A-2DDBE46A2622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{28B08333-A05C-4F72-9E1A-2DDBE46A2622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFE9FE84-C16A-4E25-9EBB-E0CAF3C7252C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Externo</t>
   </si>
@@ -60,78 +60,86 @@
     <t>Extemporano</t>
   </si>
   <si>
-    <t>Registrar Compra</t>
+    <t>Conferir mercadoria</t>
   </si>
   <si>
     <t>FB</t>
   </si>
   <si>
-    <t>Cliente solicita produto</t>
+    <t>Receber mercadoria</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Verificar mercadoria</t>
+  </si>
+  <si>
+    <t>x(1)</t>
+  </si>
+  <si>
+    <t>Devolver mercadoria</t>
+  </si>
+  <si>
+    <t>x(9)</t>
+  </si>
+  <si>
+    <t>Registrar orçamento</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Fazer orcamento</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>Cliente compra produto</t>
-  </si>
-  <si>
-    <t>x(1)</t>
-  </si>
-  <si>
-    <t>Cliente escolhe forma de pagamento</t>
-  </si>
-  <si>
-    <t>Cliente realiza pagamento</t>
-  </si>
-  <si>
-    <t>FA</t>
-  </si>
-  <si>
-    <t>Cliente cancela pedido</t>
-  </si>
-  <si>
-    <t>Gerenciar estoque</t>
-  </si>
-  <si>
-    <t>Almoxerifado confere mercadoria</t>
-  </si>
-  <si>
-    <t>Mercadoria com defeito</t>
-  </si>
-  <si>
-    <t>Conferir mercadoria</t>
-  </si>
-  <si>
-    <t>Fornecedor entrega mercadoria</t>
-  </si>
-  <si>
-    <t>Fornecedor recebe nota fiscal</t>
-  </si>
-  <si>
-    <t>Gerencia gera relatoria da mercadoria</t>
-  </si>
-  <si>
-    <t>x(2)</t>
-  </si>
-  <si>
-    <t>Fornecedor fornece mercadoria errada</t>
-  </si>
-  <si>
-    <t>Verificar vendas</t>
-  </si>
-  <si>
-    <t>Gerência consulta venda</t>
-  </si>
-  <si>
-    <t>Gerência não consegue fazer consulta</t>
+    <t>Registar compra</t>
+  </si>
+  <si>
+    <t>Receber solicitação de produto</t>
+  </si>
+  <si>
+    <t>Vender produto</t>
+  </si>
+  <si>
+    <t>Efetuar pagamento</t>
+  </si>
+  <si>
+    <t>x(6)</t>
+  </si>
+  <si>
+    <t>Cancelar produto</t>
+  </si>
+  <si>
+    <t>Fazer cancelamento</t>
+  </si>
+  <si>
+    <t>x(7)</t>
+  </si>
+  <si>
+    <t>Trocar produto</t>
+  </si>
+  <si>
+    <t>Fazer troca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -200,18 +208,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,7 +288,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J15"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,320 +658,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="8" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="6"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="16">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="2">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="17">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="6"/>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="2">
+      <c r="C11" s="7">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="6"/>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2">
-        <v>12</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="6"/>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="5"/>
+      <c r="E12" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>